<commit_message>
updated with new models and tests
</commit_message>
<xml_diff>
--- a/dev/ML_model_performance.xlsx
+++ b/dev/ML_model_performance.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\phil\Documents\GitHub\point_cloud_vegetation_filtering\dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8059201-F671-4B17-99B3-03C0B3AAB139}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84F352A4-3665-4E11-909A-828480BD9E72}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1545" yWindow="2460" windowWidth="18345" windowHeight="12045" activeTab="2" xr2:uid="{8DCF5AFF-D886-48A3-80E0-141B4EF1DBE8}"/>
+    <workbookView xWindow="4215" yWindow="450" windowWidth="22575" windowHeight="11100" xr2:uid="{8DCF5AFF-D886-48A3-80E0-141B4EF1DBE8}"/>
   </bookViews>
   <sheets>
     <sheet name="analysis" sheetId="1" r:id="rId1"/>
@@ -18574,8 +18574,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98F6A66E-88A0-4AD5-8234-0F09C8AD5240}">
   <dimension ref="B1:AP36"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="F36" sqref="F36"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="N37" sqref="N37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21110,11 +21110,26 @@
       <c r="I34" s="40" t="s">
         <v>57</v>
       </c>
-      <c r="J34" s="1"/>
-      <c r="K34" s="2"/>
-      <c r="L34" s="2"/>
-      <c r="M34" s="3"/>
-      <c r="N34" s="3"/>
+      <c r="J34" s="1">
+        <f>AVERAGE(C33:C34)</f>
+        <v>6</v>
+      </c>
+      <c r="K34" s="2">
+        <f>AVERAGE(D33:D34)</f>
+        <v>0.49990000000000001</v>
+      </c>
+      <c r="L34" s="2">
+        <f>AVERAGE(E33:E34)</f>
+        <v>0.50029999999999997</v>
+      </c>
+      <c r="M34" s="3">
+        <f>AVERAGE(F33:F34)</f>
+        <v>587</v>
+      </c>
+      <c r="N34" s="3">
+        <f>AVERAGE(G33:G34)</f>
+        <v>441</v>
+      </c>
       <c r="W34" s="22"/>
       <c r="X34" s="22"/>
       <c r="Y34" s="22"/>
@@ -21198,11 +21213,26 @@
       <c r="I36" s="40" t="s">
         <v>59</v>
       </c>
-      <c r="J36" s="1"/>
-      <c r="K36" s="2"/>
-      <c r="L36" s="2"/>
-      <c r="M36" s="3"/>
-      <c r="N36" s="3"/>
+      <c r="J36" s="1">
+        <f>AVERAGE(C35:C36)</f>
+        <v>10.5</v>
+      </c>
+      <c r="K36" s="2">
+        <f>AVERAGE(D35:D36)</f>
+        <v>0.95155000000000001</v>
+      </c>
+      <c r="L36" s="2">
+        <f>AVERAGE(E35:E36)</f>
+        <v>0.95250000000000001</v>
+      </c>
+      <c r="M36" s="3">
+        <f>AVERAGE(F35:F36)</f>
+        <v>928</v>
+      </c>
+      <c r="N36" s="3">
+        <f>AVERAGE(G35:G36)</f>
+        <v>417</v>
+      </c>
       <c r="W36" s="22"/>
       <c r="X36" s="22"/>
       <c r="Y36" s="22"/>
@@ -22144,7 +22174,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52BD5609-9B8B-4518-8E54-BE8192B1625C}">
   <dimension ref="A1:H32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>

</xml_diff>